<commit_message>
accepted the changes for final version
</commit_message>
<xml_diff>
--- a/Data/Simulation Data/Simulation Results.xlsx
+++ b/Data/Simulation Data/Simulation Results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40980" yWindow="4680" windowWidth="31360" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="57640" yWindow="11100" windowWidth="31360" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Adaptive Soalr Facade</t>
   </si>
@@ -203,7 +203,13 @@
     <t>Raw Data</t>
   </si>
   <si>
-    <t>Processed</t>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Geneva</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,7 @@
   <dimension ref="A4:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1017,7 +1023,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1088,6 +1094,128 @@
       <c r="F17" s="2">
         <f t="shared" ref="F17" si="6">SUM(F14:F16)</f>
         <v>668.50943586638414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>187.50321353282945</v>
+      </c>
+      <c r="C20">
+        <v>213.19707002935795</v>
+      </c>
+      <c r="F20">
+        <v>185.15471421997933</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>2079.8640022203717</v>
+      </c>
+      <c r="C21">
+        <v>799.89439384586956</v>
+      </c>
+      <c r="F21">
+        <v>420.62746351700548</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>104.62679985624089</v>
+      </c>
+      <c r="C22">
+        <v>108.5460830047442</v>
+      </c>
+      <c r="F22">
+        <v>107.964882204067</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2371.9940156094417</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1121.6375468799718</v>
+      </c>
+      <c r="F23" s="2">
+        <v>713.7470599410517</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>365.76173582189318</v>
+      </c>
+      <c r="C26">
+        <v>415.8325987766292</v>
+      </c>
+      <c r="F26">
+        <v>369.54191716892848</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>1124.8438800999168</v>
+      </c>
+      <c r="C27">
+        <v>352.86847729782613</v>
+      </c>
+      <c r="F27">
+        <v>188.50041448898779</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>128.18094614216687</v>
+      </c>
+      <c r="C28">
+        <v>137.51049324455718</v>
+      </c>
+      <c r="F28">
+        <v>131.3938665503843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1618.7865620639768</v>
+      </c>
+      <c r="C29" s="2">
+        <v>906.2115693190126</v>
+      </c>
+      <c r="F29" s="2">
+        <v>689.43619820830054</v>
       </c>
     </row>
     <row r="35" spans="3:10">
@@ -1135,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B17:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1170,19 +1298,19 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="D18">
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="E18">
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="F18">
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="G18">
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
@@ -1347,23 +1475,23 @@
       </c>
       <c r="C25" s="2">
         <f>C23*C18</f>
-        <v>670.83333333333314</v>
+        <v>593.74999999999977</v>
       </c>
       <c r="D25" s="2">
         <f>D18*D24*D23</f>
-        <v>469.58333333333314</v>
+        <v>415.62499999999983</v>
       </c>
       <c r="E25" s="2">
         <f>E18*E24*E23</f>
-        <v>412.76374999999979</v>
+        <v>365.33437499999985</v>
       </c>
       <c r="F25" s="2">
         <f>F18*F24*F23</f>
-        <v>412.76374999999979</v>
+        <v>365.33437499999985</v>
       </c>
       <c r="G25" s="2">
         <f>G18*G24*G23</f>
-        <v>412.76374999999979</v>
+        <v>365.33437499999985</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>17</v>
@@ -1395,23 +1523,23 @@
       </c>
       <c r="C27">
         <f>C26*C25</f>
-        <v>73.791666666666643</v>
+        <v>65.312499999999972</v>
       </c>
       <c r="D27">
         <f>D26*D25</f>
-        <v>51.654166666666647</v>
+        <v>45.718749999999979</v>
       </c>
       <c r="E27">
         <f>E26*E25</f>
-        <v>45.404012499999979</v>
+        <v>40.186781249999981</v>
       </c>
       <c r="F27">
         <f>F26*F25</f>
-        <v>41.27637499999998</v>
+        <v>36.533437499999984</v>
       </c>
       <c r="G27">
         <f>G26*G25</f>
-        <v>57.786924999999975</v>
+        <v>51.146812499999982</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
@@ -1486,23 +1614,23 @@
       </c>
       <c r="C31" s="2">
         <f>C27*C28*C29*C30</f>
-        <v>518.19459999999981</v>
+        <v>458.65049999999979</v>
       </c>
       <c r="D31" s="2">
         <f>D27*D28*D29*D30</f>
-        <v>471.08599999999979</v>
+        <v>416.95499999999976</v>
       </c>
       <c r="E31" s="2">
         <f>E27*E28*E29*E30</f>
-        <v>690.14098999999965</v>
+        <v>610.83907499999964</v>
       </c>
       <c r="F31" s="2">
         <f>F27*F28*F29*F30</f>
-        <v>627.40089999999964</v>
+        <v>555.3082499999997</v>
       </c>
       <c r="G31" s="2">
         <f>G27*G28*G29*G30</f>
-        <v>878.36125999999956</v>
+        <v>777.43154999999967</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>35</v>
@@ -1519,7 +1647,7 @@
       </c>
       <c r="C37" s="6">
         <f>C18</f>
-        <v>966</v>
+        <v>855</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1558,7 +1686,7 @@
       </c>
       <c r="C40" s="6">
         <f>C25</f>
-        <v>670.83333333333314</v>
+        <v>593.74999999999977</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1609,8 +1737,8 @@
         <v>46</v>
       </c>
       <c r="C44" s="6">
-        <f t="shared" ref="C44:G44" si="0">C31</f>
-        <v>518.19459999999981</v>
+        <f t="shared" ref="C44" si="0">C31</f>
+        <v>458.65049999999979</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>

</xml_diff>